<commit_message>
C128 / MacOS tools
</commit_message>
<xml_diff>
--- a/Documents/misc/Wi-Fi Modem BOM.xlsx
+++ b/Documents/misc/Wi-Fi Modem BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t>Part#</t>
   </si>
@@ -72,9 +72,6 @@
     <t>http://www.digikey.ca/product-detail/en/0/S5751-10-ND</t>
   </si>
   <si>
-    <t>4116R-1-331LF</t>
-  </si>
-  <si>
     <t>Socket for RN-XV</t>
   </si>
   <si>
@@ -84,12 +81,6 @@
     <t>Resistor Network</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.digikey.ca/product-detail/en/0/4116R-1-331LF-ND </t>
-  </si>
-  <si>
-    <t>Current Limiting (330 Ohm)</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -222,9 +213,6 @@
     <t>Separate Component</t>
   </si>
   <si>
-    <t>Leif Bloomquist</t>
-  </si>
-  <si>
     <t>AAA Scrap Dogs Unlimited</t>
   </si>
   <si>
@@ -244,6 +232,15 @@
   </si>
   <si>
     <t>https://www.creatroninc.com</t>
+  </si>
+  <si>
+    <t>Hackvana</t>
+  </si>
+  <si>
+    <t>Current Limiting 100 Ohm)</t>
+  </si>
+  <si>
+    <t>4116R-1-101LF</t>
   </si>
 </sst>
 </file>
@@ -665,7 +662,7 @@
   <dimension ref="A2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,10 +679,10 @@
   <sheetData>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -697,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
@@ -714,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -723,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -737,7 +734,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -746,13 +743,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -760,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -769,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -783,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -795,13 +792,13 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -809,20 +806,20 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G7" s="7"/>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -830,7 +827,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -839,16 +836,16 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,51 +856,49 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -911,19 +906,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -931,16 +926,16 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -948,22 +943,22 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -971,7 +966,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3">
         <v>2</v>
@@ -980,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G14" t="s">
         <v>12</v>
@@ -994,16 +989,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
         <v>15</v>
@@ -1017,19 +1012,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="3">
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1037,16 +1032,16 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3">
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1054,41 +1049,40 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
-    <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H4" r:id="rId3"/>
-    <hyperlink ref="H18" r:id="rId4"/>
-    <hyperlink ref="H6" r:id="rId5"/>
-    <hyperlink ref="H5" r:id="rId6"/>
-    <hyperlink ref="H8" r:id="rId7"/>
-    <hyperlink ref="H13" r:id="rId8"/>
-    <hyperlink ref="H11" r:id="rId9"/>
-    <hyperlink ref="H3" r:id="rId10"/>
-    <hyperlink ref="H10" r:id="rId11"/>
-    <hyperlink ref="H16" r:id="rId12"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H18" r:id="rId3"/>
+    <hyperlink ref="H6" r:id="rId4"/>
+    <hyperlink ref="H5" r:id="rId5"/>
+    <hyperlink ref="H8" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H11" r:id="rId8"/>
+    <hyperlink ref="H3" r:id="rId9"/>
+    <hyperlink ref="H10" r:id="rId10"/>
+    <hyperlink ref="H16" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>